<commit_message>
update xlsl font size
</commit_message>
<xml_diff>
--- a/documents/SOIL_LIB.xlsx
+++ b/documents/SOIL_LIB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xHM\example_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xHM\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64BAD7C-01F8-4A2C-A7A9-7F53FD89A166}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A0E0CE-A5F1-43EE-8B0B-B15F332B74EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22760" windowHeight="5700" xr2:uid="{6982937E-D96A-42A5-9BE5-C5D8CBCA0A5D}"/>
   </bookViews>
@@ -152,7 +152,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF1F2328"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -178,14 +178,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,606 +507,610 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="4"/>
+    <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="8.7265625" style="4"/>
+    <col min="8" max="8" width="22.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>36</v>
       </c>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>29.9</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>42</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>48.8</v>
       </c>
-      <c r="F2" s="1">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="F2" s="2">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2">
         <v>0.12</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>7.7999999999999999E-4</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2">
         <v>1.36</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>48.2</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="2">
         <v>11.4</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="2">
         <v>0.40500000000000003</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="2">
         <v>0.46799999999999997</v>
       </c>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>27.8</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>41.6</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>53.2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>10.9</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>3.81E-3</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="2">
         <v>1.24</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
         <v>49.2</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="2">
         <v>10.4</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="2">
         <v>0.49</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="2">
         <v>0.32400000000000001</v>
       </c>
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>29.9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>42</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>48.8</v>
       </c>
-      <c r="F4" s="1">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="F4" s="2">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2">
         <v>0.12</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>7.7999999999999999E-4</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="2">
         <v>1.36</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="2">
         <v>48.2</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="2">
         <v>11.4</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="2">
         <v>0.40500000000000003</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="2">
         <v>0.46799999999999997</v>
       </c>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>21</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>37.9</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>51</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>4</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>0.17</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>5.9299999999999995E-3</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="2">
         <v>1.3</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="2">
         <v>47.7</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="2">
         <v>7.75</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="2">
         <v>0.35600000000000004</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="2">
         <v>0.61699999999999999</v>
       </c>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>21.3</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>35</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>47.2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>7.5</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>4.5599999999999998E-3</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="2">
         <v>1.4</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="2">
         <v>47.6</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="2">
         <v>8.52</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="2">
         <v>0.63</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="2">
         <v>0.26300000000000001</v>
       </c>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>6.3</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>31.6</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>48.2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>1.5</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>0.25</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <v>1.8949999999999998E-2</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="2">
         <v>1.37</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="2">
         <v>52</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="2">
         <v>7.8</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="2">
         <v>0.63800000000000001</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="2">
         <v>0.75900000000000001</v>
       </c>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>13.7</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>32.1</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>48.2</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <v>1.5</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>0.18</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>1.2189999999999999E-2</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="2">
         <v>1.37</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="2">
         <v>48.5</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="2">
         <v>5.3</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="2">
         <v>0.78599999999999992</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="2">
         <v>0.75900000000000001</v>
       </c>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>26</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>37.1</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>44</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>5.6</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <v>0.11</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>8.3999999999999993E-4</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="2">
         <v>1.48</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="2">
         <v>42.6</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="2">
         <v>10.4</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="2">
         <v>0.153</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>12.6</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>26.7</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>45.8</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <v>2.7</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <v>1.8600000000000002E-2</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="2">
         <v>1.44</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="2">
         <v>45.1</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="2">
         <v>5.39</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="2">
         <v>0.47799999999999998</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="2">
         <v>0.35499999999999998</v>
       </c>
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>18.3</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>28.3</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>43.2</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <v>6.8</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>0.1</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>7.8399999999999997E-3</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="2">
         <v>1.51</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="2">
         <v>42</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="2">
         <v>7.12</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="2">
         <v>0.29899999999999999</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="2">
         <v>0.13500000000000001</v>
       </c>
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>8.1</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>17.899999999999999</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
         <v>45</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>0.1</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>5.0340000000000003E-2</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="2">
         <v>1.46</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="2">
         <v>43.5</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="2">
         <v>0.153</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="2">
         <v>0.14099999999999999</v>
       </c>
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>5.7</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>12.1</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
         <v>45.7</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <v>3.5</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <v>0.06</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <v>9.1260000000000008E-2</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="2">
         <v>1.44</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="2">
         <v>41</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="2">
         <v>4.38</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="2">
         <v>0.09</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="2">
         <v>3.6000000000000004E-2</v>
       </c>
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>5</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>9.4</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>46.3</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2">
         <v>2</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <v>0.04</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="2">
         <v>0.11405</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="2">
         <v>1.42</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="2">
         <v>39.5</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="2">
         <v>4.05</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="2">
         <v>0.121</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="2">
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="N14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>